<commit_message>
Swap dates and default frequency set.
</commit_message>
<xml_diff>
--- a/xll_isda_cds.xlsx
+++ b/xll_isda_cds.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kal\Source\Repos\keithalewis\xll_isda_cds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalx\source\repos\isda_cds_model\xll_isda_cds\xll_isda_cds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600CF9DB-1D00-494A-9076-88CA257C077E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,14 +33,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -85,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,6 +151,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -521,307 +521,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>2.0477874017427844E-2</c:v>
+                  <c:v>2.0479022694424476E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.046582413725373E-2</c:v>
+                  <c:v>2.0465632941256029E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0441558423625494E-2</c:v>
+                  <c:v>2.0442033410969396E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.043077014993111E-2</c:v>
+                  <c:v>2.0431466790747033E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.446059432218517E-2</c:v>
+                  <c:v>2.4766919390539988E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7873356659814608E-2</c:v>
+                  <c:v>2.8075030007503887E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0154845248417939E-2</c:v>
+                  <c:v>3.0286367797119906E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0591820051985463E-2</c:v>
+                  <c:v>3.0589767593514727E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0539373551432325E-2</c:v>
+                  <c:v>3.0537736010148198E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0498583674011703E-2</c:v>
+                  <c:v>3.0497268817017975E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0465952934524143E-2</c:v>
+                  <c:v>3.0464896206645165E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0439255825297939E-2</c:v>
+                  <c:v>3.0438410281857342E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0417008762630759E-2</c:v>
+                  <c:v>3.041633919789688E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.1518275917765459E-2</c:v>
+                  <c:v>3.1464615699908105E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.2984088834254965E-2</c:v>
+                  <c:v>3.2938531048446018E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.4256144802396138E-2</c:v>
+                  <c:v>3.4217627889381319E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.5370478693843799E-2</c:v>
+                  <c:v>3.5338136864962344E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.6354711486074054E-2</c:v>
+                  <c:v>3.63278293785807E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.72303705109851E-2</c:v>
+                  <c:v>3.720835025186231E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.8014482039500086E-2</c:v>
+                  <c:v>3.7996818854921788E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.8720689214020831E-2</c:v>
+                  <c:v>3.8706953055249516E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.9360052558703451E-2</c:v>
+                  <c:v>3.9349874047397204E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.9941633464381843E-2</c:v>
+                  <c:v>3.993469299362129E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.0472926323573466E-2</c:v>
+                  <c:v>4.0468945500936382E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.0960183218793356E-2</c:v>
+                  <c:v>4.095891807246943E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.1842301371262769E-2</c:v>
+                  <c:v>4.1843525864032616E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.3074686109715987E-2</c:v>
+                  <c:v>4.3078202773928487E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.4217082851609746E-2</c:v>
+                  <c:v>4.4222726734658879E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.5279000110483691E-2</c:v>
+                  <c:v>4.5286623440293106E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.6268652443682612E-2</c:v>
+                  <c:v>4.6278122323753612E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.7193173306435687E-2</c:v>
+                  <c:v>4.7204369784751066E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.8058787229438682E-2</c:v>
+                  <c:v>4.807160167077118E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.8870950108395927E-2</c:v>
+                  <c:v>4.8885283814579017E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.9634464288987434E-2</c:v>
+                  <c:v>4.9650227323172036E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.0353573576426225E-2</c:v>
+                  <c:v>5.0370683756185919E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.1032042139621536E-2</c:v>
+                  <c:v>5.1050424170624664E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.1673220407395748E-2</c:v>
+                  <c:v>5.1692805134746278E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.2489204425372415E-2</c:v>
+                  <c:v>5.0773468600526339E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.3670447161006329E-2</c:v>
+                  <c:v>4.7341646129006154E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.479233883230461E-2</c:v>
+                  <c:v>4.4096176012196953E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.5859242333788917E-2</c:v>
+                  <c:v>4.1022295144780951E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.6875103220763057E-2</c:v>
+                  <c:v>3.8106758369680582E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.784349843911385E-2</c:v>
+                  <c:v>3.5337648423971801E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.8767678383942368E-2</c:v>
+                  <c:v>3.2704213721803654E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.9650603328636365E-2</c:v>
+                  <c:v>3.0196729333954675E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6.0494975084206981E-2</c:v>
+                  <c:v>2.7806377386607739E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6.1303264601846097E-2</c:v>
+                  <c:v>2.5525143788556193E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.2077736112429394E-2</c:v>
+                  <c:v>2.3345728745441052E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.2820468299426002E-2</c:v>
+                  <c:v>2.126146896161818E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>6.3486737846446498E-2</c:v>
+                  <c:v>1.9658459765005361E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,7 +829,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4D10-4BC7-BEAB-A8E584B4D5CE}"/>
+              <c16:uniqueId val="{00000000-3AC1-452A-8A92-9088B599AB2C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1872,33 +1872,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D8877F-7093-4DDC-9262-75C479E7D9B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1909,13 +1910,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" cm="1">
-        <f t="array" ref="C3">_xll.JPMCDS.BUILD.IR.ZERO.CURVE(C2, F6:F10, F15:F17)</f>
-        <v>-9.2559600142467789E+61</v>
+      <c r="C3" s="3">
+        <f>_xll.JPMCDS.BUILD.IR.ZERO.CURVE(C2, F6:F10, F15:F17)</f>
+        <v>7202171</v>
       </c>
       <c r="H3" s="1">
         <f>C2</f>
@@ -1923,20 +1924,20 @@
       </c>
       <c r="I3">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H3)</f>
-        <v>2.0477874017427844E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.45">
+        <v>2.0479022694424476E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H4" s="1">
         <f>H3+$H$2</f>
         <v>43649</v>
       </c>
       <c r="I4">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H4)</f>
-        <v>2.046582413725373E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.45">
+        <v>2.0465632941256029E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1949,10 +1950,10 @@
       </c>
       <c r="I5">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H5)</f>
-        <v>2.0441558423625494E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.45">
+        <v>2.0442033410969396E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -1961,14 +1962,14 @@
       </c>
       <c r="D6" cm="1">
         <f t="array" ref="D6">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET(B6, C6)</f>
-        <v>-9.255959760630308E+61</v>
+        <v>-769478</v>
       </c>
       <c r="E6">
         <v>0.02</v>
       </c>
       <c r="F6" cm="1">
         <f t="array" ref="F6">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET.SET(D6, E6, $C$2)</f>
-        <v>-9.255959760630308E+61</v>
+        <v>-769478</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="0"/>
@@ -1976,10 +1977,10 @@
       </c>
       <c r="I6">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H6)</f>
-        <v>2.043077014993111E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.45">
+        <v>2.0431466790747033E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -1988,14 +1989,14 @@
       </c>
       <c r="D7" cm="1">
         <f t="array" ref="D7">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET(B7, C7)</f>
-        <v>-9.2559597606483575E+61</v>
+        <v>-769437</v>
       </c>
       <c r="E7">
         <v>0.02</v>
       </c>
       <c r="F7" cm="1">
         <f t="array" ref="F7">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET.SET(D7, E7, $C$2)</f>
-        <v>-9.2559597606483575E+61</v>
+        <v>-769437</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
@@ -2003,10 +2004,10 @@
       </c>
       <c r="I7">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H7)</f>
-        <v>2.446059432218517E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.45">
+        <v>2.4766919390539988E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>3</v>
       </c>
@@ -2015,14 +2016,14 @@
       </c>
       <c r="D8" cm="1">
         <f t="array" ref="D8">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET(B8, C8)</f>
-        <v>-9.2559597606322079E+61</v>
+        <v>-39378</v>
       </c>
       <c r="E8">
         <v>0.02</v>
       </c>
       <c r="F8" cm="1">
         <f t="array" ref="F8">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET.SET(D8, E8, $C$2)</f>
-        <v>-9.2559597606322079E+61</v>
+        <v>-39378</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="0"/>
@@ -2030,10 +2031,10 @@
       </c>
       <c r="I8">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H8)</f>
-        <v>2.7873356659814608E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.45">
+        <v>2.8075030007503887E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -2042,14 +2043,14 @@
       </c>
       <c r="D9" cm="1">
         <f t="array" ref="D9">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET(B9, C9)</f>
-        <v>-9.2559597606311392E+61</v>
+        <v>-769485</v>
       </c>
       <c r="E9">
         <v>0.03</v>
       </c>
       <c r="F9" cm="1">
         <f t="array" ref="F9">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET.SET(D9, E9, $C$2)</f>
-        <v>-9.2559597606311392E+61</v>
+        <v>-769485</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
@@ -2057,10 +2058,10 @@
       </c>
       <c r="I9">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H9)</f>
-        <v>3.0154845248417939E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.0286367797119906E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -2069,14 +2070,14 @@
       </c>
       <c r="D10" cm="1">
         <f t="array" ref="D10">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET(B10, C10)</f>
-        <v>-9.2559597606335142E+61</v>
+        <v>-769482</v>
       </c>
       <c r="E10">
         <v>0.03</v>
       </c>
       <c r="F10" cm="1">
         <f t="array" ref="F10">_xll.JPMCDS.INSTRUMENT.MONEY.MARKET.SET(D10, E10, $C$2)</f>
-        <v>-9.2559597606335142E+61</v>
+        <v>-769482</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="0"/>
@@ -2084,40 +2085,40 @@
       </c>
       <c r="I10">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H10)</f>
-        <v>3.0591820051985463E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.0589767593514727E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H11" s="1">
         <f t="shared" si="0"/>
         <v>43859</v>
       </c>
       <c r="I11">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H11)</f>
-        <v>3.0539373551432325E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.0537736010148198E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H12" s="1">
         <f t="shared" si="0"/>
         <v>43889</v>
       </c>
       <c r="I12">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H12)</f>
-        <v>3.0498583674011703E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.0497268817017975E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H13" s="1">
         <f t="shared" si="0"/>
         <v>43919</v>
       </c>
       <c r="I13">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H13)</f>
-        <v>3.0465952934524143E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.0464896206645165E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -2127,10 +2128,10 @@
       </c>
       <c r="I14">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H14)</f>
-        <v>3.0439255825297939E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.0438410281857342E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2</v>
       </c>
@@ -2139,14 +2140,14 @@
       </c>
       <c r="D15" cm="1">
         <f t="array" ref="D15">_xll.JPMCDS.INSTRUMENT.INTEREST.RATE.SWAP(B15,C15)</f>
-        <v>-9.2559597630992775E+61</v>
+        <v>520517</v>
       </c>
       <c r="E15">
         <v>0.04</v>
       </c>
       <c r="F15" cm="1">
         <f t="array" ref="F15">_xll.JPMCDS.INSTRUMENT.INTEREST.RATE.SWAP.SET(D15, E15, $C$2)</f>
-        <v>-9.2559597630992775E+61</v>
+        <v>520517</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="0"/>
@@ -2154,10 +2155,10 @@
       </c>
       <c r="I15">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H15)</f>
-        <v>3.0417008762630759E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.041633919789688E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>3</v>
       </c>
@@ -2166,14 +2167,14 @@
       </c>
       <c r="D16" cm="1">
         <f t="array" ref="D16">_xll.JPMCDS.INSTRUMENT.INTEREST.RATE.SWAP(B16,C16)</f>
-        <v>-9.2559597631028399E+61</v>
+        <v>520453</v>
       </c>
       <c r="E16">
         <v>0.05</v>
       </c>
       <c r="F16" cm="1">
         <f t="array" ref="F16">_xll.JPMCDS.INSTRUMENT.INTEREST.RATE.SWAP.SET(D16, E16, $C$2)</f>
-        <v>-9.2559597631028399E+61</v>
+        <v>520453</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="0"/>
@@ -2181,10 +2182,10 @@
       </c>
       <c r="I16">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H16)</f>
-        <v>3.1518275917765459E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.1464615699908105E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>4</v>
       </c>
@@ -2193,14 +2194,14 @@
       </c>
       <c r="D17" cm="1">
         <f t="array" ref="D17">_xll.JPMCDS.INSTRUMENT.INTEREST.RATE.SWAP(B17,C17)</f>
-        <v>-9.2559597631029769E+61</v>
+        <v>520477</v>
       </c>
       <c r="E17">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="F17" cm="1">
         <f t="array" ref="F17">_xll.JPMCDS.INSTRUMENT.INTEREST.RATE.SWAP.SET(D17, E17, $C$2)</f>
-        <v>-9.2559597631029769E+61</v>
+        <v>520477</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="0"/>
@@ -2208,867 +2209,867 @@
       </c>
       <c r="I17">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H17)</f>
-        <v>3.2984088834254965E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.2938531048446018E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H18" s="1">
         <f t="shared" si="0"/>
         <v>44069</v>
       </c>
       <c r="I18">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H18)</f>
-        <v>3.4256144802396138E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.4217627889381319E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H19" s="1">
         <f t="shared" si="0"/>
         <v>44099</v>
       </c>
       <c r="I19">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H19)</f>
-        <v>3.5370478693843799E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.5338136864962344E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H20" s="1">
         <f t="shared" si="0"/>
         <v>44129</v>
       </c>
       <c r="I20">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H20)</f>
-        <v>3.6354711486074054E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.63278293785807E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H21" s="1">
         <f t="shared" si="0"/>
         <v>44159</v>
       </c>
       <c r="I21">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H21)</f>
-        <v>3.72303705109851E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.720835025186231E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H22" s="1">
         <f t="shared" si="0"/>
         <v>44189</v>
       </c>
       <c r="I22">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H22)</f>
-        <v>3.8014482039500086E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.7996818854921788E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H23" s="1">
         <f t="shared" si="0"/>
         <v>44219</v>
       </c>
       <c r="I23">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H23)</f>
-        <v>3.8720689214020831E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.8706953055249516E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H24" s="1">
         <f t="shared" si="0"/>
         <v>44249</v>
       </c>
       <c r="I24">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H24)</f>
-        <v>3.9360052558703451E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.9349874047397204E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H25" s="1">
         <f t="shared" si="0"/>
         <v>44279</v>
       </c>
       <c r="I25">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H25)</f>
-        <v>3.9941633464381843E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+        <v>3.993469299362129E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H26" s="1">
         <f t="shared" si="0"/>
         <v>44309</v>
       </c>
       <c r="I26">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H26)</f>
-        <v>4.0472926323573466E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
+        <v>4.0468945500936382E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H27" s="1">
         <f t="shared" si="0"/>
         <v>44339</v>
       </c>
       <c r="I27">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H27)</f>
-        <v>4.0960183218793356E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.45">
+        <v>4.095891807246943E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H28" s="1">
         <f t="shared" si="0"/>
         <v>44369</v>
       </c>
       <c r="I28">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H28)</f>
-        <v>4.1842301371262769E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+        <v>4.1843525864032616E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H29" s="1">
         <f t="shared" si="0"/>
         <v>44399</v>
       </c>
       <c r="I29">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H29)</f>
-        <v>4.3074686109715987E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+        <v>4.3078202773928487E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H30" s="1">
         <f t="shared" si="0"/>
         <v>44429</v>
       </c>
       <c r="I30">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H30)</f>
-        <v>4.4217082851609746E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+        <v>4.4222726734658879E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H31" s="1">
         <f t="shared" si="0"/>
         <v>44459</v>
       </c>
       <c r="I31">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H31)</f>
-        <v>4.5279000110483691E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+        <v>4.5286623440293106E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H32" s="1">
         <f t="shared" si="0"/>
         <v>44489</v>
       </c>
       <c r="I32">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H32)</f>
-        <v>4.6268652443682612E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
+        <v>4.6278122323753612E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" s="1">
         <f t="shared" si="0"/>
         <v>44519</v>
       </c>
       <c r="I33">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H33)</f>
-        <v>4.7193173306435687E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
+        <v>4.7204369784751066E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H34" s="1">
         <f t="shared" si="0"/>
         <v>44549</v>
       </c>
       <c r="I34">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H34)</f>
-        <v>4.8058787229438682E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
+        <v>4.807160167077118E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H35" s="1">
         <f t="shared" si="0"/>
         <v>44579</v>
       </c>
       <c r="I35">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H35)</f>
-        <v>4.8870950108395927E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
+        <v>4.8885283814579017E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H36" s="1">
         <f t="shared" si="0"/>
         <v>44609</v>
       </c>
       <c r="I36">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H36)</f>
-        <v>4.9634464288987434E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
+        <v>4.9650227323172036E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H37" s="1">
         <f t="shared" si="0"/>
         <v>44639</v>
       </c>
       <c r="I37">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H37)</f>
-        <v>5.0353573576426225E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
+        <v>5.0370683756185919E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H38" s="1">
         <f t="shared" si="0"/>
         <v>44669</v>
       </c>
       <c r="I38">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H38)</f>
-        <v>5.1032042139621536E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
+        <v>5.1050424170624664E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H39" s="1">
         <f t="shared" si="0"/>
         <v>44699</v>
       </c>
       <c r="I39">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H39)</f>
-        <v>5.1673220407395748E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
+        <v>5.1692805134746278E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H40" s="1">
         <f t="shared" si="0"/>
         <v>44729</v>
       </c>
       <c r="I40">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H40)</f>
-        <v>5.2489204425372415E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
+        <v>5.0773468600526339E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H41" s="1">
         <f t="shared" si="0"/>
         <v>44759</v>
       </c>
       <c r="I41">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H41)</f>
-        <v>5.3670447161006329E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
+        <v>4.7341646129006154E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H42" s="1">
         <f t="shared" si="0"/>
         <v>44789</v>
       </c>
       <c r="I42">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H42)</f>
-        <v>5.479233883230461E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.45">
+        <v>4.4096176012196953E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H43" s="1">
         <f t="shared" si="0"/>
         <v>44819</v>
       </c>
       <c r="I43">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H43)</f>
-        <v>5.5859242333788917E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.45">
+        <v>4.1022295144780951E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H44" s="1">
         <f t="shared" si="0"/>
         <v>44849</v>
       </c>
       <c r="I44">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H44)</f>
-        <v>5.6875103220763057E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.45">
+        <v>3.8106758369680582E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H45" s="1">
         <f t="shared" si="0"/>
         <v>44879</v>
       </c>
       <c r="I45">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H45)</f>
-        <v>5.784349843911385E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.45">
+        <v>3.5337648423971801E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H46" s="1">
         <f t="shared" si="0"/>
         <v>44909</v>
       </c>
       <c r="I46">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H46)</f>
-        <v>5.8767678383942368E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.45">
+        <v>3.2704213721803654E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H47" s="1">
         <f t="shared" si="0"/>
         <v>44939</v>
       </c>
       <c r="I47">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H47)</f>
-        <v>5.9650603328636365E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.45">
+        <v>3.0196729333954675E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H48" s="1">
         <f t="shared" si="0"/>
         <v>44969</v>
       </c>
       <c r="I48">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H48)</f>
-        <v>6.0494975084206981E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.45">
+        <v>2.7806377386607739E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H49" s="1">
         <f t="shared" si="0"/>
         <v>44999</v>
       </c>
       <c r="I49">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H49)</f>
-        <v>6.1303264601846097E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.45">
+        <v>2.5525143788556193E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H50" s="1">
         <f t="shared" si="0"/>
         <v>45029</v>
       </c>
       <c r="I50">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H50)</f>
-        <v>6.2077736112429394E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.45">
+        <v>2.3345728745441052E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H51" s="1">
         <f t="shared" si="0"/>
         <v>45059</v>
       </c>
       <c r="I51">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H51)</f>
-        <v>6.2820468299426002E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.45">
+        <v>2.126146896161818E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H52" s="1">
         <f t="shared" si="0"/>
         <v>45089</v>
       </c>
       <c r="I52">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H52)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H53" s="1">
         <f t="shared" si="0"/>
         <v>45119</v>
       </c>
       <c r="I53">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H53)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H54" s="1">
         <f t="shared" si="0"/>
         <v>45149</v>
       </c>
       <c r="I54">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H54)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H55" s="1">
         <f t="shared" si="0"/>
         <v>45179</v>
       </c>
       <c r="I55">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H55)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H56" s="1">
         <f t="shared" si="0"/>
         <v>45209</v>
       </c>
       <c r="I56">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H56)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H57" s="1">
         <f t="shared" si="0"/>
         <v>45239</v>
       </c>
       <c r="I57">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H57)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H58" s="1">
         <f t="shared" si="0"/>
         <v>45269</v>
       </c>
       <c r="I58">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H58)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H59" s="1">
         <f t="shared" si="0"/>
         <v>45299</v>
       </c>
       <c r="I59">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H59)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H60" s="1">
         <f t="shared" si="0"/>
         <v>45329</v>
       </c>
       <c r="I60">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H60)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H61" s="1">
         <f t="shared" si="0"/>
         <v>45359</v>
       </c>
       <c r="I61">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H61)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H62" s="1">
         <f t="shared" si="0"/>
         <v>45389</v>
       </c>
       <c r="I62">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H62)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H63" s="1">
         <f t="shared" si="0"/>
         <v>45419</v>
       </c>
       <c r="I63">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H63)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H64" s="1">
         <f t="shared" si="0"/>
         <v>45449</v>
       </c>
       <c r="I64">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H64)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H65" s="1">
         <f t="shared" si="0"/>
         <v>45479</v>
       </c>
       <c r="I65">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H65)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H66" s="1">
         <f t="shared" si="0"/>
         <v>45509</v>
       </c>
       <c r="I66">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H66)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H67" s="1">
         <f t="shared" si="0"/>
         <v>45539</v>
       </c>
       <c r="I67">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H67)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H68" s="1">
         <f t="shared" si="0"/>
         <v>45569</v>
       </c>
       <c r="I68">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H68)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H69" s="1">
         <f t="shared" ref="H69:H103" si="1">H68+$H$2</f>
         <v>45599</v>
       </c>
       <c r="I69">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H69)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H70" s="1">
         <f t="shared" si="1"/>
         <v>45629</v>
       </c>
       <c r="I70">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H70)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H71" s="1">
         <f t="shared" si="1"/>
         <v>45659</v>
       </c>
       <c r="I71">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H71)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H72" s="1">
         <f t="shared" si="1"/>
         <v>45689</v>
       </c>
       <c r="I72">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H72)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H73" s="1">
         <f t="shared" si="1"/>
         <v>45719</v>
       </c>
       <c r="I73">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H73)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H74" s="1">
         <f t="shared" si="1"/>
         <v>45749</v>
       </c>
       <c r="I74">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H74)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H75" s="1">
         <f t="shared" si="1"/>
         <v>45779</v>
       </c>
       <c r="I75">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H75)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H76" s="1">
         <f t="shared" si="1"/>
         <v>45809</v>
       </c>
       <c r="I76">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H76)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H77" s="1">
         <f t="shared" si="1"/>
         <v>45839</v>
       </c>
       <c r="I77">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H77)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H78" s="1">
         <f t="shared" si="1"/>
         <v>45869</v>
       </c>
       <c r="I78">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H78)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H79" s="1">
         <f t="shared" si="1"/>
         <v>45899</v>
       </c>
       <c r="I79">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H79)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H80" s="1">
         <f t="shared" si="1"/>
         <v>45929</v>
       </c>
       <c r="I80">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H80)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H81" s="1">
         <f t="shared" si="1"/>
         <v>45959</v>
       </c>
       <c r="I81">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H81)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H82" s="1">
         <f t="shared" si="1"/>
         <v>45989</v>
       </c>
       <c r="I82">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H82)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H83" s="1">
         <f t="shared" si="1"/>
         <v>46019</v>
       </c>
       <c r="I83">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H83)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H84" s="1">
         <f t="shared" si="1"/>
         <v>46049</v>
       </c>
       <c r="I84">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H84)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H85" s="1">
         <f t="shared" si="1"/>
         <v>46079</v>
       </c>
       <c r="I85">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H85)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H86" s="1">
         <f t="shared" si="1"/>
         <v>46109</v>
       </c>
       <c r="I86">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H86)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H87" s="1">
         <f t="shared" si="1"/>
         <v>46139</v>
       </c>
       <c r="I87">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H87)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H88" s="1">
         <f t="shared" si="1"/>
         <v>46169</v>
       </c>
       <c r="I88">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H88)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H89" s="1">
         <f t="shared" si="1"/>
         <v>46199</v>
       </c>
       <c r="I89">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H89)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H90" s="1">
         <f t="shared" si="1"/>
         <v>46229</v>
       </c>
       <c r="I90">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H90)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H91" s="1">
         <f t="shared" si="1"/>
         <v>46259</v>
       </c>
       <c r="I91">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H91)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H92" s="1">
         <f t="shared" si="1"/>
         <v>46289</v>
       </c>
       <c r="I92">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H92)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H93" s="1">
         <f t="shared" si="1"/>
         <v>46319</v>
       </c>
       <c r="I93">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H93)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H94" s="1">
         <f t="shared" si="1"/>
         <v>46349</v>
       </c>
       <c r="I94">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H94)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H95" s="1">
         <f t="shared" si="1"/>
         <v>46379</v>
       </c>
       <c r="I95">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H95)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H96" s="1">
         <f t="shared" si="1"/>
         <v>46409</v>
       </c>
       <c r="I96">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H96)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H97" s="1">
         <f t="shared" si="1"/>
         <v>46439</v>
       </c>
       <c r="I97">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H97)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H98" s="1">
         <f t="shared" si="1"/>
         <v>46469</v>
       </c>
       <c r="I98">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H98)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H99" s="1">
         <f t="shared" si="1"/>
         <v>46499</v>
       </c>
       <c r="I99">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H99)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H100" s="1">
         <f t="shared" si="1"/>
         <v>46529</v>
       </c>
       <c r="I100">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H100)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H101" s="1">
         <f t="shared" si="1"/>
         <v>46559</v>
       </c>
       <c r="I101">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H101)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H102" s="1">
         <f t="shared" si="1"/>
         <v>46589</v>
       </c>
       <c r="I102">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H102)</f>
-        <v>6.3486737846446498E-2</v>
-      </c>
-    </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.45">
+        <v>1.9658459765005361E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H103" s="1">
         <f t="shared" si="1"/>
         <v>46619</v>
       </c>
       <c r="I103">
         <f>_xll.JPMCDS.TCURVE.RATE($C$3, H103)</f>
-        <v>6.3486737846446498E-2</v>
+        <v>1.9658459765005361E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>